<commit_message>
refactor: Unless column deleted
</commit_message>
<xml_diff>
--- a/DATA/TradeLog.xlsx
+++ b/DATA/TradeLog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이세령\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINJUN KWAK\Documents\github\KOSDAQ-Gap-Strategy\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7425" tabRatio="598"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7425" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -1806,11 +1806,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2004,7 +2004,7 @@
         <v>501551</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" ref="L6:L39" si="0">SUM(J6:K6)</f>
+        <f t="shared" ref="L6:L31" si="0">SUM(J6:K6)</f>
         <v>501551</v>
       </c>
       <c r="M6" s="14"/>
@@ -2995,119 +2995,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O31" s="8">
-        <f t="shared" ref="O30:O37" si="20">D32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="I32" s="11">
-        <f t="shared" ref="I32" si="21">ROUNDDOWN(C32*E32*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O32" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="I33" s="11">
-        <f t="shared" ref="I33" si="22">ROUNDDOWN(D33*E33*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="2"/>
-      <c r="I34" s="11">
-        <f t="shared" ref="I34" si="23">ROUNDDOWN(C34*E34*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
-      <c r="I35" s="11">
-        <f t="shared" ref="I35" si="24">ROUNDDOWN(D35*E35*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="2"/>
-      <c r="I36" s="11">
-        <f t="shared" ref="I36" si="25">ROUNDDOWN(C36*E36*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O36" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
-      <c r="I37" s="11">
-        <f t="shared" ref="I37" si="26">ROUNDDOWN(D37*E37*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O37" s="8">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I38" s="11">
-        <f t="shared" ref="I38" si="27">ROUNDDOWN(D38*E38*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I39" s="11">
-        <f t="shared" ref="I39" si="28">ROUNDDOWN(C39*E39*0.00011,)</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="O31" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -3135,7 +3025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3484,7 +3374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">

</xml_diff>